<commit_message>
CCSB Loads: N and S Abutments, wy2010-15: updated Menlo Lab Data folder, v35; added SSC model results for 8_wy2010-15; updated pTHg model results for 8_wy2010-15; updated Sigma Plot folder for 8_wy2010-15; added site folder for 8_wy2010-15 N_Abutment; for S_Abutment wy_2010-15:  added AQUARIUS files, updated Q+WQ worksheet,  added SSC to rloadest folder,  replaced pTHg rloadest folder (reran with corrected values); updated Loads Progress sheet, updated Google Drive tracking log.
</commit_message>
<xml_diff>
--- a/2018-19_CCSB_LoadsData_WY2010-2018/Sites/S_Abutment_11452800/8_wy2010-2015/8_rloadest/8_pTHg/8_Excel for Text Files/pTHg_SWeirR.xlsx
+++ b/2018-19_CCSB_LoadsData_WY2010-2018/Sites/S_Abutment_11452800/8_wy2010-2015/8_rloadest/8_pTHg/8_Excel for Text Files/pTHg_SWeirR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slrose\R\2018-19_CCSB_LoadsData_WY2010-2018\Sites\S_Abutment_11452800\8_wy2010-2015\8_rloadest\8_pTHg\8_Excel for Text Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C80CFC89-F5B0-4B5D-9616-8C35915025D7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9430951D-057B-4476-9A70-3B9D953E5B41}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5BFDCA5C-ACDB-4827-B2A0-E0EF925E6C2A}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="15165" windowHeight="12360" xr2:uid="{E0566B44-3D78-49C4-83A1-A678BE6D8F0E}"/>
   </bookViews>
   <sheets>
     <sheet name="8_pTHg" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
     <numFmt numFmtId="165" formatCode="h:mm;@"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,26 +71,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC3F9EB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -105,16 +92,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,7 +416,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E9AEB71-ECBC-495D-8968-F4DF19B9778F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1984B4A2-F45B-415F-8FF0-C039BF1AD7CD}">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
@@ -477,27 +465,27 @@
       <c r="A3" s="4">
         <v>40542</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="5">
         <v>0.63194444444444442</v>
       </c>
-      <c r="C3" s="5">
-        <v>733</v>
-      </c>
-      <c r="D3" s="6">
-        <v>44.6</v>
+      <c r="C3" s="6">
+        <v>777.11456666666663</v>
+      </c>
+      <c r="D3" s="7">
+        <v>44.57</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>40547</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="5">
         <v>0.65972222222222199</v>
       </c>
-      <c r="C4" s="5">
-        <v>776</v>
-      </c>
-      <c r="D4" s="6">
+      <c r="C4" s="6">
+        <v>747.88316666666674</v>
+      </c>
+      <c r="D4" s="7">
         <v>7</v>
       </c>
     </row>
@@ -505,111 +493,111 @@
       <c r="A5" s="4">
         <v>40602</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="5">
         <v>0.42361111111111099</v>
       </c>
-      <c r="C5" s="5">
-        <v>44</v>
-      </c>
-      <c r="D5" s="6">
-        <v>8.6999999999999993</v>
+      <c r="C5" s="6">
+        <v>46.699286666666666</v>
+      </c>
+      <c r="D5" s="7">
+        <v>8.67</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>40617</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="5">
         <v>0.453125</v>
       </c>
-      <c r="C6" s="7">
-        <v>1036</v>
-      </c>
-      <c r="D6" s="6">
-        <v>3.4</v>
+      <c r="C6" s="6">
+        <v>1036.4580000000001</v>
+      </c>
+      <c r="D6" s="7">
+        <v>3.3899999999999997</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>40619</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="5">
         <v>0.47222222222222199</v>
       </c>
-      <c r="C7" s="5">
-        <v>1900</v>
-      </c>
-      <c r="D7" s="6">
-        <v>6.2</v>
+      <c r="C7" s="6">
+        <v>1800.2513333333334</v>
+      </c>
+      <c r="D7" s="7">
+        <v>6.22</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>40621</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="5">
         <v>0.79861111111111105</v>
       </c>
-      <c r="C8" s="5">
-        <v>4120</v>
-      </c>
-      <c r="D8" s="6">
-        <v>68.3</v>
+      <c r="C8" s="6">
+        <v>4720.614333333333</v>
+      </c>
+      <c r="D8" s="7">
+        <v>68.319999999999993</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>40623</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="5">
         <v>0.38194444444444398</v>
       </c>
-      <c r="C9" s="5">
-        <v>9380</v>
-      </c>
-      <c r="D9" s="8">
-        <v>193</v>
+      <c r="C9" s="6">
+        <v>9718.2923333333329</v>
+      </c>
+      <c r="D9" s="6">
+        <v>192.66</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>40624</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="5">
         <v>0.33333333333333298</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="6">
         <v>5300</v>
       </c>
-      <c r="D10" s="6">
-        <v>49.9</v>
+      <c r="D10" s="7">
+        <v>49.92</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>40627</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="5">
         <v>0.46527777777777801</v>
       </c>
-      <c r="C11" s="5">
-        <v>10900</v>
-      </c>
-      <c r="D11" s="8">
-        <v>215</v>
+      <c r="C11" s="6">
+        <v>11009.033333333335</v>
+      </c>
+      <c r="D11" s="6">
+        <v>214.7</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>40637</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="5">
         <v>0.36111111111111099</v>
       </c>
-      <c r="C12" s="5">
-        <v>3120</v>
-      </c>
-      <c r="D12" s="6">
+      <c r="C12" s="6">
+        <v>3863.7781545391545</v>
+      </c>
+      <c r="D12" s="7">
         <v>12.8</v>
       </c>
     </row>
@@ -617,168 +605,168 @@
       <c r="A13" s="4">
         <v>41246</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="5">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="6">
         <v>1900</v>
       </c>
-      <c r="D13" s="8">
-        <v>228</v>
+      <c r="D13" s="6">
+        <v>227.94</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>41248</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="5">
         <v>0.59027777777777779</v>
       </c>
-      <c r="C14" s="5">
-        <v>274</v>
-      </c>
-      <c r="D14" s="6">
-        <v>40.9</v>
+      <c r="C14" s="6">
+        <v>273.50110000000001</v>
+      </c>
+      <c r="D14" s="7">
+        <v>40.869999999999997</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>41266</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="5">
         <v>0.45833333333333331</v>
       </c>
-      <c r="C15" s="5">
-        <v>1750</v>
-      </c>
-      <c r="D15" s="6">
-        <v>92</v>
+      <c r="C15" s="6">
+        <v>1750.377</v>
+      </c>
+      <c r="D15" s="7">
+        <v>92.01</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>41267</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="5">
         <v>0.52777777777777779</v>
       </c>
-      <c r="C16" s="5">
-        <v>7340</v>
-      </c>
-      <c r="D16" s="8">
-        <v>250</v>
+      <c r="C16" s="6">
+        <v>7377.5926666666664</v>
+      </c>
+      <c r="D16" s="6">
+        <v>250.21</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>41270</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="5">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C17" s="5">
-        <v>960</v>
-      </c>
-      <c r="D17" s="6">
-        <v>21.1</v>
+      <c r="C17" s="6">
+        <v>960.28459999999995</v>
+      </c>
+      <c r="D17" s="7">
+        <v>21.05</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>41985</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="5">
         <v>0.65972222222222221</v>
       </c>
-      <c r="C18" s="3">
-        <v>5362</v>
-      </c>
-      <c r="D18" s="8">
-        <v>739</v>
+      <c r="C18" s="6">
+        <v>5361.9653333333335</v>
+      </c>
+      <c r="D18" s="6">
+        <v>739.14</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>41986</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="5">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C19" s="3">
-        <v>3030</v>
-      </c>
-      <c r="D19" s="8">
-        <v>241</v>
+      <c r="C19" s="6">
+        <v>3029.8440000000001</v>
+      </c>
+      <c r="D19" s="6">
+        <v>240.77</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>41988</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="5">
         <v>0.45833333333333331</v>
       </c>
-      <c r="C20" s="3">
-        <v>912</v>
-      </c>
-      <c r="D20" s="8">
-        <v>184</v>
+      <c r="C20" s="6">
+        <v>911.6893</v>
+      </c>
+      <c r="D20" s="6">
+        <v>183.81</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>41989</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="5">
         <v>0.74305555555555547</v>
       </c>
-      <c r="C21" s="3">
-        <v>2524</v>
-      </c>
-      <c r="D21" s="6">
-        <v>36</v>
+      <c r="C21" s="6">
+        <v>2524.3130000000001</v>
+      </c>
+      <c r="D21" s="7">
+        <v>35.979999999999997</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>41993</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="5">
         <v>0.62534722222222228</v>
       </c>
-      <c r="C22" s="3">
-        <v>2097</v>
-      </c>
-      <c r="D22" s="6">
-        <v>25.8</v>
+      <c r="C22" s="6">
+        <v>2096.8220000000001</v>
+      </c>
+      <c r="D22" s="7">
+        <v>25.75</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>42044</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="5">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C23" s="3">
-        <v>1171</v>
-      </c>
-      <c r="D23" s="8">
-        <v>131</v>
+      <c r="C23" s="6">
+        <v>1171.289</v>
+      </c>
+      <c r="D23" s="6">
+        <v>131.22</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>42045</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="5">
         <v>0.5625</v>
       </c>
-      <c r="C24" s="3">
-        <v>1228</v>
-      </c>
-      <c r="D24" s="6">
-        <v>81.8</v>
+      <c r="C24" s="6">
+        <v>1228.3489999999999</v>
+      </c>
+      <c r="D24" s="7">
+        <v>81.760000000000005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>